<commit_message>
Core64 LED Matrix V0.3 release to manufacturing
</commit_message>
<xml_diff>
--- a/Electronic Design/Core64 LM v0.3/Core64_LM_V0.3_Gerbers/Core64 LM v0.3_BOM.xlsx
+++ b/Electronic Design/Core64 LM v0.3/Core64_LM_V0.3_Gerbers/Core64 LM v0.3_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/Core64 LM v0.2/Core64_LM_V0.2_Gerbers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/Core64 LM v0.3/Core64_LM_V0.3_Gerbers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57E2C68-52E4-1A46-97F5-4D8FB2AD6DDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0924F18F-F8B8-0041-9F13-884DB1ECF8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,19 +86,19 @@
     <t>0603_C</t>
   </si>
   <si>
-    <t>C187860</t>
-  </si>
-  <si>
-    <t>C114592</t>
-  </si>
-  <si>
-    <t>WS2813B-B</t>
-  </si>
-  <si>
     <t>C1-8</t>
   </si>
   <si>
     <t>D1-64</t>
+  </si>
+  <si>
+    <t>WS2813C</t>
+  </si>
+  <si>
+    <t>C194323</t>
+  </si>
+  <si>
+    <t>C14663</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -497,13 +497,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29" customHeight="1">
@@ -511,13 +511,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
         <v>5050</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>